<commit_message>
64 bytes limit added
</commit_message>
<xml_diff>
--- a/db_groups/MO-231db.xlsx
+++ b/db_groups/MO-231db.xlsx
@@ -448,12 +448,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Алгебра</t>
+          <t>Матанализ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>13.02.24 14:25</t>
+          <t>13.01.24 14:00</t>
         </is>
       </c>
     </row>

</xml_diff>